<commit_message>
Falta descargar archivos en splash
</commit_message>
<xml_diff>
--- a/documentos/datos.xlsx
+++ b/documentos/datos.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/io/Documents/Desarrollo/prototipo2/documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itanortegaortega/Documents/Desarrollo/prototipo2/documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="460" windowWidth="15420" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="es" sheetId="2" r:id="rId1"/>
     <sheet name="en" sheetId="1" r:id="rId2"/>
     <sheet name="signos1" sheetId="4" r:id="rId3"/>
-    <sheet name="Datos Signos" sheetId="3" r:id="rId4"/>
-    <sheet name="compatibilidad" sheetId="6" r:id="rId5"/>
-    <sheet name="compatibiliad resultado" sheetId="7" r:id="rId6"/>
-    <sheet name="diario" sheetId="5" r:id="rId7"/>
+    <sheet name="iniciales" sheetId="8" r:id="rId4"/>
+    <sheet name="Datos Signos" sheetId="3" r:id="rId5"/>
+    <sheet name="compatibilidad" sheetId="6" r:id="rId6"/>
+    <sheet name="compatibiliad resultado" sheetId="7" r:id="rId7"/>
+    <sheet name="diario" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="595">
   <si>
     <t>app_name</t>
   </si>
@@ -1770,6 +1771,54 @@
   </si>
   <si>
     <t>piscis_acuario=39%</t>
+  </si>
+  <si>
+    <t>compatibilidad.json</t>
+  </si>
+  <si>
+    <t>signos.json</t>
+  </si>
+  <si>
+    <t>acuario.png</t>
+  </si>
+  <si>
+    <t>aries.png</t>
+  </si>
+  <si>
+    <t>cancer.png</t>
+  </si>
+  <si>
+    <t>capricornio.png</t>
+  </si>
+  <si>
+    <t>escorpio.png</t>
+  </si>
+  <si>
+    <t>geminis.png</t>
+  </si>
+  <si>
+    <t>leo.png</t>
+  </si>
+  <si>
+    <t>libra.png</t>
+  </si>
+  <si>
+    <t>piscis.png</t>
+  </si>
+  <si>
+    <t>sagitario.png</t>
+  </si>
+  <si>
+    <t>taruro.png</t>
+  </si>
+  <si>
+    <t>virgo.png</t>
+  </si>
+  <si>
+    <t>archivos</t>
+  </si>
+  <si>
+    <t>imágenes</t>
   </si>
 </sst>
 </file>
@@ -4627,7 +4676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4735,6 +4784,235 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1" t="s">
+        <v>579</v>
+      </c>
+      <c r="D1" t="str">
+        <f>B1&amp;"["&amp;A1&amp;"]   archivo="&amp;C1</f>
+        <v>archivos[0]   archivo=compatibilidad.json</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C2" t="s">
+        <v>580</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D14" si="0">B2&amp;"["&amp;A2&amp;"]   archivo="&amp;C2</f>
+        <v>archivos[1]   archivo=signos.json</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>594</v>
+      </c>
+      <c r="C3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[0]   archivo=acuario.png</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>594</v>
+      </c>
+      <c r="C4" t="s">
+        <v>582</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[1]   archivo=aries.png</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>594</v>
+      </c>
+      <c r="C5" t="s">
+        <v>583</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[2]   archivo=cancer.png</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>594</v>
+      </c>
+      <c r="C6" t="s">
+        <v>584</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[3]   archivo=capricornio.png</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>594</v>
+      </c>
+      <c r="C7" t="s">
+        <v>585</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[4]   archivo=escorpio.png</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>594</v>
+      </c>
+      <c r="C8" t="s">
+        <v>586</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[5]   archivo=geminis.png</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>594</v>
+      </c>
+      <c r="C9" t="s">
+        <v>587</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[6]   archivo=leo.png</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>594</v>
+      </c>
+      <c r="C10" t="s">
+        <v>588</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[7]   archivo=libra.png</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>594</v>
+      </c>
+      <c r="C11" t="s">
+        <v>589</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[8]   archivo=piscis.png</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>594</v>
+      </c>
+      <c r="C12" t="s">
+        <v>590</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[9]   archivo=sagitario.png</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>594</v>
+      </c>
+      <c r="C13" t="s">
+        <v>591</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[10]   archivo=taruro.png</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>594</v>
+      </c>
+      <c r="C14" t="s">
+        <v>592</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[11]   archivo=virgo.png</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F131"/>
   <sheetViews>
@@ -7211,7 +7489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
@@ -8711,7 +8989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A144"/>
   <sheetViews>
@@ -9446,7 +9724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>

</xml_diff>

<commit_message>
numeros de la suerte
</commit_message>
<xml_diff>
--- a/documentos/datos.xlsx
+++ b/documentos/datos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="es" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="616">
   <si>
     <t>app_name</t>
   </si>
@@ -1855,6 +1855,33 @@
   </si>
   <si>
     <t>virgo_fondo.png</t>
+  </si>
+  <si>
+    <t>iucesmag.png</t>
+  </si>
+  <si>
+    <t>caldas.png</t>
+  </si>
+  <si>
+    <t>baloto.png</t>
+  </si>
+  <si>
+    <t>chance.png</t>
+  </si>
+  <si>
+    <t>num.png</t>
+  </si>
+  <si>
+    <t>circulofn.png</t>
+  </si>
+  <si>
+    <t>numeros</t>
+  </si>
+  <si>
+    <t>pnl</t>
+  </si>
+  <si>
+    <t>pnl1; pnl2</t>
   </si>
 </sst>
 </file>
@@ -4710,108 +4737,147 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -4821,10 +4887,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4859,7 +4925,7 @@
         <v>580</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D26" si="0">B2&amp;"["&amp;A2&amp;"]   archivo="&amp;C2</f>
+        <f t="shared" ref="D2:D32" si="0">B2&amp;"["&amp;A2&amp;"]   archivo="&amp;C2</f>
         <v>archivos[1]   archivo=signos.json</v>
       </c>
     </row>
@@ -5221,6 +5287,96 @@
       <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>imágenes[23]   archivo=virgo_fondo.png</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>593</v>
+      </c>
+      <c r="C27" t="s">
+        <v>607</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[24]   archivo=iucesmag.png</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>593</v>
+      </c>
+      <c r="C28" t="s">
+        <v>608</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[25]   archivo=caldas.png</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>593</v>
+      </c>
+      <c r="C29" t="s">
+        <v>609</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[26]   archivo=baloto.png</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>593</v>
+      </c>
+      <c r="C30" t="s">
+        <v>610</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[27]   archivo=chance.png</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>593</v>
+      </c>
+      <c r="C31" t="s">
+        <v>611</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[28]   archivo=num.png</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>593</v>
+      </c>
+      <c r="C32" t="s">
+        <v>612</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>imágenes[29]   archivo=circulofn.png</v>
       </c>
     </row>
   </sheetData>
@@ -9942,595 +10098,2696 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D2:D37"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <f>C1+B1</f>
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f ca="1">RANDBETWEEN(1,4)</f>
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f ca="1">RANDBETWEEN(5,7)</f>
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <f ca="1">RANDBETWEEN(8,9)</f>
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <f ca="1">RANDBETWEEN(1000,9999)</f>
+        <v>5453</v>
+      </c>
+      <c r="E2">
+        <f ca="1">RANDBETWEEN(100000,999999)</f>
+        <v>616810</v>
+      </c>
+      <c r="F2" t="str">
+        <f ca="1">A2&amp;","&amp;B2&amp;" y "&amp;C2&amp;"; "&amp;D2&amp;"; "&amp;E2</f>
+        <v>4,5 y 9; 5453; 616810</v>
+      </c>
+      <c r="K2" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f t="shared" ref="A3:A62" ca="1" si="0">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B62" ca="1" si="1">RANDBETWEEN(5,7)</f>
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C62" ca="1" si="2">RANDBETWEEN(8,9)</f>
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D62" ca="1" si="3">RANDBETWEEN(1000,9999)</f>
+        <v>9402</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E62" ca="1" si="4">RANDBETWEEN(100000,999999)</f>
+        <v>330111</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F62" ca="1" si="5">A3&amp;","&amp;B3&amp;" y "&amp;C3&amp;"; "&amp;D3&amp;"; "&amp;E3</f>
+        <v>2,6 y 9; 9402; 330111</v>
+      </c>
+      <c r="G3" t="str">
+        <f>VLOOKUP(H3,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
-      <c r="B2" t="str">
-        <f>VLOOKUP(A2,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I3" t="str">
+        <f>VLOOKUP(H3,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>aries</v>
       </c>
-      <c r="C2" t="s">
+      <c r="J3" t="s">
         <v>433</v>
       </c>
-      <c r="D2" t="str">
-        <f>IF(C2="es","  "&amp;B2&amp;"_"&amp;C2&amp;"="&amp;VLOOKUP(B2&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C2="en","  "&amp;B2&amp;"_"&amp;C2&amp;"="&amp;VLOOKUP(B2&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A2&amp;"]"))</f>
+      <c r="K3" t="str">
+        <f>IF(J3="es","  "&amp;I3&amp;"_"&amp;J3&amp;"="&amp;VLOOKUP(I3&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J3="en","  "&amp;I3&amp;"_"&amp;J3&amp;"="&amp;VLOOKUP(I3&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J3="indice",$K$2&amp;"["&amp;H3&amp;"]",IF(J3="pnl","  pnl="&amp;G3,"  num="&amp;F3))))</f>
         <v>horoscopo[0]</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="3"/>
+        <v>6827</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="4"/>
+        <v>349433</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,6 y 9; 6827; 349433</v>
+      </c>
+      <c r="G4" t="str">
+        <f>VLOOKUP(H4,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="B3" t="str">
-        <f>VLOOKUP(A3,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I4" t="str">
+        <f>VLOOKUP(H4,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>aries</v>
       </c>
-      <c r="C3" t="s">
+      <c r="J4" t="s">
+        <v>613</v>
+      </c>
+      <c r="K4" t="str">
+        <f ca="1">IF(J4="es","  "&amp;I4&amp;"_"&amp;J4&amp;"="&amp;VLOOKUP(I4&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J4="en","  "&amp;I4&amp;"_"&amp;J4&amp;"="&amp;VLOOKUP(I4&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J4="indice",$K$2&amp;"["&amp;H4&amp;"]",IF(J4="pnl","  pnl="&amp;G4,"  num="&amp;F4))))</f>
+        <v xml:space="preserve">  num=3,6 y 9; 6827; 349433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="3"/>
+        <v>6041</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="4"/>
+        <v>673213</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,5 y 8; 6041; 673213</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(H5,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="str">
+        <f>VLOOKUP(H5,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>aries</v>
+      </c>
+      <c r="J5" t="s">
+        <v>614</v>
+      </c>
+      <c r="K5" t="str">
+        <f>IF(J5="es","  "&amp;I5&amp;"_"&amp;J5&amp;"="&amp;VLOOKUP(I5&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J5="en","  "&amp;I5&amp;"_"&amp;J5&amp;"="&amp;VLOOKUP(I5&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J5="indice",$K$2&amp;"["&amp;H5&amp;"]",IF(J5="pnl","  pnl="&amp;G5,"  num="&amp;F5))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="3"/>
+        <v>3042</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="4"/>
+        <v>985349</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 9; 3042; 985349</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP(H6,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="str">
+        <f>VLOOKUP(H6,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>aries</v>
+      </c>
+      <c r="J6" t="s">
         <v>126</v>
       </c>
-      <c r="D3" t="str">
-        <f>IF(C3="es","  "&amp;B3&amp;"_"&amp;C3&amp;"="&amp;VLOOKUP(B3&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C3="en","  "&amp;B3&amp;"_"&amp;C3&amp;"="&amp;VLOOKUP(B3&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A3&amp;"]"))</f>
+      <c r="K6" t="str">
+        <f>IF(J6="es","  "&amp;I6&amp;"_"&amp;J6&amp;"="&amp;VLOOKUP(I6&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J6="en","  "&amp;I6&amp;"_"&amp;J6&amp;"="&amp;VLOOKUP(I6&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J6="indice",$K$2&amp;"["&amp;H6&amp;"]",IF(J6="pnl","  pnl="&amp;G6,"  num="&amp;F6))))</f>
         <v xml:space="preserve">  aries_es=Los planetas te respaldan todo lo que hace falta corta tus ataduras y ve al fondo de las cosas hoy. Los planetas te están creando cierta resistencia para los temas de la carrera puedes pensar que no progresas tanto como quisieras. No tienes paciencia para ponerte en línea hoy. Tu atención debe volcarse hacia un proyecto creativo o de negocios las condiciones son particularmente propicias ahora y no debes perder la oportunidad. Vas aprisa en tu carrera y te vuelve loco lo que haces Tienes tiempo para algo más y corres peligro de que las cosas pierdan el equilibrio.</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="3"/>
+        <v>8723</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="4"/>
+        <v>563421</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,7 y 8; 8723; 563421</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(H7,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
-      <c r="B4" t="str">
-        <f>VLOOKUP(A4,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I7" t="str">
+        <f>VLOOKUP(H7,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>aries</v>
       </c>
-      <c r="C4" t="s">
+      <c r="J7" t="s">
         <v>432</v>
       </c>
-      <c r="D4" t="str">
-        <f>IF(C4="es","  "&amp;B4&amp;"_"&amp;C4&amp;"="&amp;VLOOKUP(B4&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C4="en","  "&amp;B4&amp;"_"&amp;C4&amp;"="&amp;VLOOKUP(B4&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A4&amp;"]"))</f>
+      <c r="K7" t="str">
+        <f>IF(J7="es","  "&amp;I7&amp;"_"&amp;J7&amp;"="&amp;VLOOKUP(I7&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J7="en","  "&amp;I7&amp;"_"&amp;J7&amp;"="&amp;VLOOKUP(I7&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J7="indice",$K$2&amp;"["&amp;H7&amp;"]",IF(J7="pnl","  pnl="&amp;G7,"  num="&amp;F7))))</f>
         <v xml:space="preserve">  aries_en=Planets support you all you need to cut your ties and go to the bottom of things today. The planets are creating some resistance for the subjects of the race you can think that you do not progress as much as you would like. You do not have the patience to get online today. Your attention should be turned towards a creative or business project. The conditions are particularly propitious now and you should not miss the opportunity. You go fast in your career and it drives you crazy what you do. You have time for something else and you run the risk of things losing their balance.</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="3"/>
+        <v>5118</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="4"/>
+        <v>493152</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,5 y 8; 5118; 493152</v>
+      </c>
+      <c r="G8" t="str">
+        <f>VLOOKUP(H8,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
-      <c r="B5" t="str">
-        <f>VLOOKUP(A5,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I8" t="str">
+        <f>VLOOKUP(H8,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>tauro</v>
       </c>
-      <c r="C5" t="s">
+      <c r="J8" t="s">
         <v>433</v>
       </c>
-      <c r="D5" t="str">
-        <f>IF(C5="es","  "&amp;B5&amp;"_"&amp;C5&amp;"="&amp;VLOOKUP(B5&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C5="en","  "&amp;B5&amp;"_"&amp;C5&amp;"="&amp;VLOOKUP(B5&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A5&amp;"]"))</f>
+      <c r="K8" t="str">
+        <f>IF(J8="es","  "&amp;I8&amp;"_"&amp;J8&amp;"="&amp;VLOOKUP(I8&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J8="en","  "&amp;I8&amp;"_"&amp;J8&amp;"="&amp;VLOOKUP(I8&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J8="indice",$K$2&amp;"["&amp;H8&amp;"]",IF(J8="pnl","  pnl="&amp;G8,"  num="&amp;F8))))</f>
         <v>horoscopo[1]</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="3"/>
+        <v>7572</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="4"/>
+        <v>908457</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,5 y 9; 7572; 908457</v>
+      </c>
+      <c r="G9" t="str">
+        <f>VLOOKUP(H9,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H9">
         <v>1</v>
       </c>
-      <c r="B6" t="str">
-        <f>VLOOKUP(A6,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I9" t="str">
+        <f>VLOOKUP(H9,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>tauro</v>
       </c>
-      <c r="C6" t="s">
+      <c r="J9" t="s">
+        <v>613</v>
+      </c>
+      <c r="K9" t="str">
+        <f ca="1">IF(J9="es","  "&amp;I9&amp;"_"&amp;J9&amp;"="&amp;VLOOKUP(I9&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J9="en","  "&amp;I9&amp;"_"&amp;J9&amp;"="&amp;VLOOKUP(I9&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J9="indice",$K$2&amp;"["&amp;H9&amp;"]",IF(J9="pnl","  pnl="&amp;G9,"  num="&amp;F9))))</f>
+        <v xml:space="preserve">  num=3,5 y 9; 7572; 908457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="3"/>
+        <v>4059</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="4"/>
+        <v>368826</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,5 y 8; 4059; 368826</v>
+      </c>
+      <c r="G10" t="str">
+        <f>VLOOKUP(H10,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="str">
+        <f>VLOOKUP(H10,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>tauro</v>
+      </c>
+      <c r="J10" t="s">
+        <v>614</v>
+      </c>
+      <c r="K10" t="str">
+        <f>IF(J10="es","  "&amp;I10&amp;"_"&amp;J10&amp;"="&amp;VLOOKUP(I10&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J10="en","  "&amp;I10&amp;"_"&amp;J10&amp;"="&amp;VLOOKUP(I10&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J10="indice",$K$2&amp;"["&amp;H10&amp;"]",IF(J10="pnl","  pnl="&amp;G10,"  num="&amp;F10))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="3"/>
+        <v>7022</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="4"/>
+        <v>357716</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,5 y 9; 7022; 357716</v>
+      </c>
+      <c r="G11" t="str">
+        <f>VLOOKUP(H11,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="str">
+        <f>VLOOKUP(H11,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>tauro</v>
+      </c>
+      <c r="J11" t="s">
         <v>126</v>
       </c>
-      <c r="D6" t="str">
-        <f>IF(C6="es","  "&amp;B6&amp;"_"&amp;C6&amp;"="&amp;VLOOKUP(B6&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C6="en","  "&amp;B6&amp;"_"&amp;C6&amp;"="&amp;VLOOKUP(B6&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A6&amp;"]"))</f>
+      <c r="K11" t="str">
+        <f>IF(J11="es","  "&amp;I11&amp;"_"&amp;J11&amp;"="&amp;VLOOKUP(I11&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J11="en","  "&amp;I11&amp;"_"&amp;J11&amp;"="&amp;VLOOKUP(I11&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J11="indice",$K$2&amp;"["&amp;H11&amp;"]",IF(J11="pnl","  pnl="&amp;G11,"  num="&amp;F11))))</f>
         <v xml:space="preserve">  tauro_es=Se honesto contigo mismo y con los demás hoy independientemente de las presiones que sientas. Sólo pensar en dinero te causa disgusto pero meter la cabeza en la arena no es una solución. Tu ánimo vuelve luego de un pequeño periodo de incertidumbre Se optimista y tus planes de carrera despegarán. Es posible que tenga que descubrir algún engaño o fraude dentro de su lugar de trabajo, por lo que es importante estar alerta y tener un plan de acción. La cuadratura que hacen la Luna y Marte no te pone las cosas fáciles en este sentido.</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="3"/>
+        <v>6038</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="4"/>
+        <v>456633</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,5 y 8; 6038; 456633</v>
+      </c>
+      <c r="G12" t="str">
+        <f>VLOOKUP(H12,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H12">
         <v>1</v>
       </c>
-      <c r="B7" t="str">
-        <f>VLOOKUP(A7,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I12" t="str">
+        <f>VLOOKUP(H12,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>tauro</v>
       </c>
-      <c r="C7" t="s">
+      <c r="J12" t="s">
         <v>432</v>
       </c>
-      <c r="D7" t="str">
-        <f>IF(C7="es","  "&amp;B7&amp;"_"&amp;C7&amp;"="&amp;VLOOKUP(B7&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C7="en","  "&amp;B7&amp;"_"&amp;C7&amp;"="&amp;VLOOKUP(B7&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A7&amp;"]"))</f>
+      <c r="K12" t="str">
+        <f>IF(J12="es","  "&amp;I12&amp;"_"&amp;J12&amp;"="&amp;VLOOKUP(I12&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J12="en","  "&amp;I12&amp;"_"&amp;J12&amp;"="&amp;VLOOKUP(I12&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J12="indice",$K$2&amp;"["&amp;H12&amp;"]",IF(J12="pnl","  pnl="&amp;G12,"  num="&amp;F12))))</f>
         <v xml:space="preserve">  tauro_en=Be honest with yourself and with others today regardless of the pressures you feel. Just thinking about money causes you disgust but putting your head in the sand is not a solution. Your mood returns after a short period of uncertainty. Be optimistic and your career plans will take off. You may have to discover some deception or fraud within your workplace, so it is important to be alert and have an action plan. The square made by the Moon and Mars does not make things easy for you in this regard.</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="3"/>
+        <v>5609</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="4"/>
+        <v>995038</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,6 y 8; 5609; 995038</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(H13,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H13">
         <v>2</v>
       </c>
-      <c r="B8" t="str">
-        <f>VLOOKUP(A8,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I13" t="str">
+        <f>VLOOKUP(H13,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>geminis</v>
       </c>
-      <c r="C8" t="s">
+      <c r="J13" t="s">
         <v>433</v>
       </c>
-      <c r="D8" t="str">
-        <f>IF(C8="es","  "&amp;B8&amp;"_"&amp;C8&amp;"="&amp;VLOOKUP(B8&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C8="en","  "&amp;B8&amp;"_"&amp;C8&amp;"="&amp;VLOOKUP(B8&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A8&amp;"]"))</f>
+      <c r="K13" t="str">
+        <f>IF(J13="es","  "&amp;I13&amp;"_"&amp;J13&amp;"="&amp;VLOOKUP(I13&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J13="en","  "&amp;I13&amp;"_"&amp;J13&amp;"="&amp;VLOOKUP(I13&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J13="indice",$K$2&amp;"["&amp;H13&amp;"]",IF(J13="pnl","  pnl="&amp;G13,"  num="&amp;F13))))</f>
         <v>horoscopo[2]</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="3"/>
+        <v>6412</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="4"/>
+        <v>718273</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,6 y 8; 6412; 718273</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(H14,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H14">
         <v>2</v>
       </c>
-      <c r="B9" t="str">
-        <f>VLOOKUP(A9,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I14" t="str">
+        <f>VLOOKUP(H14,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>geminis</v>
       </c>
-      <c r="C9" t="s">
+      <c r="J14" t="s">
+        <v>613</v>
+      </c>
+      <c r="K14" t="str">
+        <f ca="1">IF(J14="es","  "&amp;I14&amp;"_"&amp;J14&amp;"="&amp;VLOOKUP(I14&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J14="en","  "&amp;I14&amp;"_"&amp;J14&amp;"="&amp;VLOOKUP(I14&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J14="indice",$K$2&amp;"["&amp;H14&amp;"]",IF(J14="pnl","  pnl="&amp;G14,"  num="&amp;F14))))</f>
+        <v xml:space="preserve">  num=3,6 y 8; 6412; 718273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="3"/>
+        <v>6457</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="4"/>
+        <v>393322</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,5 y 9; 6457; 393322</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(H15,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15" t="str">
+        <f>VLOOKUP(H15,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>geminis</v>
+      </c>
+      <c r="J15" t="s">
+        <v>614</v>
+      </c>
+      <c r="K15" t="str">
+        <f>IF(J15="es","  "&amp;I15&amp;"_"&amp;J15&amp;"="&amp;VLOOKUP(I15&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J15="en","  "&amp;I15&amp;"_"&amp;J15&amp;"="&amp;VLOOKUP(I15&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J15="indice",$K$2&amp;"["&amp;H15&amp;"]",IF(J15="pnl","  pnl="&amp;G15,"  num="&amp;F15))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="3"/>
+        <v>7814</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="4"/>
+        <v>276431</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 9; 7814; 276431</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(H16,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="str">
+        <f>VLOOKUP(H16,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>geminis</v>
+      </c>
+      <c r="J16" t="s">
         <v>126</v>
       </c>
-      <c r="D9" t="str">
-        <f>IF(C9="es","  "&amp;B9&amp;"_"&amp;C9&amp;"="&amp;VLOOKUP(B9&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C9="en","  "&amp;B9&amp;"_"&amp;C9&amp;"="&amp;VLOOKUP(B9&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A9&amp;"]"))</f>
+      <c r="K16" t="str">
+        <f>IF(J16="es","  "&amp;I16&amp;"_"&amp;J16&amp;"="&amp;VLOOKUP(I16&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J16="en","  "&amp;I16&amp;"_"&amp;J16&amp;"="&amp;VLOOKUP(I16&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J16="indice",$K$2&amp;"["&amp;H16&amp;"]",IF(J16="pnl","  pnl="&amp;G16,"  num="&amp;F16))))</f>
         <v xml:space="preserve">  geminis_es=Hay buenos prospectos para asumir un reto a largo plazo No importa la difícil que sea, serás capaz de salir adelante. Es momento de aceptar que loes tiempos han cambiado Ya la pelota no está en el mismo patio, Las reglas son nuevas y te las tienes que aprender de memoria. Una inesperada oportunidad puede aparecer en una situación profesional, significando esto que debes estar preparado para saltar hacia cualquier oportunidad. Si sigues manteniendo tu fe en ti mismo con tus logros a la vista las cosas se conciliarán y no podrán salirte mal. Y no lo hará por amor, sino por orgullo puro y duro.</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="3"/>
+        <v>7004</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="4"/>
+        <v>261229</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,7 y 9; 7004; 261229</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(H17,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="B10" t="str">
-        <f>VLOOKUP(A10,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I17" t="str">
+        <f>VLOOKUP(H17,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>geminis</v>
       </c>
-      <c r="C10" t="s">
+      <c r="J17" t="s">
         <v>432</v>
       </c>
-      <c r="D10" t="str">
-        <f>IF(C10="es","  "&amp;B10&amp;"_"&amp;C10&amp;"="&amp;VLOOKUP(B10&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C10="en","  "&amp;B10&amp;"_"&amp;C10&amp;"="&amp;VLOOKUP(B10&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A10&amp;"]"))</f>
+      <c r="K17" t="str">
+        <f>IF(J17="es","  "&amp;I17&amp;"_"&amp;J17&amp;"="&amp;VLOOKUP(I17&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J17="en","  "&amp;I17&amp;"_"&amp;J17&amp;"="&amp;VLOOKUP(I17&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J17="indice",$K$2&amp;"["&amp;H17&amp;"]",IF(J17="pnl","  pnl="&amp;G17,"  num="&amp;F17))))</f>
         <v xml:space="preserve">  geminis_en=There are good prospects to take on a long-term challenge No matter how difficult it may be, you will be able to get ahead. It\'s time to accept that times have changed. The ball is not in the same yard anymore. The rules are new and you have to learn them by heart. An unexpected opportunity can appear in a professional situation, meaning that you must be prepared to jump to any opportunity. If you keep your faith in yourself with your achievements in sight things will be reconciled and can not go wrong. And he will not do it out of love, but out of pure and hard pride.</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="B11" t="str">
-        <f>VLOOKUP(A11,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="B18">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="3"/>
+        <v>2945</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="4"/>
+        <v>213344</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,5 y 8; 2945; 213344</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(H18,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18" t="str">
+        <f>VLOOKUP(H18,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>cancer</v>
       </c>
-      <c r="C11" t="s">
+      <c r="J18" t="s">
         <v>433</v>
       </c>
-      <c r="D11" t="str">
-        <f>IF(C11="es","  "&amp;B11&amp;"_"&amp;C11&amp;"="&amp;VLOOKUP(B11&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C11="en","  "&amp;B11&amp;"_"&amp;C11&amp;"="&amp;VLOOKUP(B11&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A11&amp;"]"))</f>
+      <c r="K18" t="str">
+        <f>IF(J18="es","  "&amp;I18&amp;"_"&amp;J18&amp;"="&amp;VLOOKUP(I18&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J18="en","  "&amp;I18&amp;"_"&amp;J18&amp;"="&amp;VLOOKUP(I18&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J18="indice",$K$2&amp;"["&amp;H18&amp;"]",IF(J18="pnl","  pnl="&amp;G18,"  num="&amp;F18))))</f>
         <v>horoscopo[3]</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="3"/>
+        <v>2634</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="4"/>
+        <v>939264</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,7 y 8; 2634; 939264</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP(H19,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H19">
         <v>3</v>
       </c>
-      <c r="B12" t="str">
-        <f>VLOOKUP(A12,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I19" t="str">
+        <f>VLOOKUP(H19,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>cancer</v>
       </c>
-      <c r="C12" t="s">
+      <c r="J19" t="s">
+        <v>613</v>
+      </c>
+      <c r="K19" t="str">
+        <f ca="1">IF(J19="es","  "&amp;I19&amp;"_"&amp;J19&amp;"="&amp;VLOOKUP(I19&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J19="en","  "&amp;I19&amp;"_"&amp;J19&amp;"="&amp;VLOOKUP(I19&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J19="indice",$K$2&amp;"["&amp;H19&amp;"]",IF(J19="pnl","  pnl="&amp;G19,"  num="&amp;F19))))</f>
+        <v xml:space="preserve">  num=2,7 y 8; 2634; 939264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="3"/>
+        <v>7098</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="4"/>
+        <v>636283</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 8; 7098; 636283</v>
+      </c>
+      <c r="G20" t="str">
+        <f>VLOOKUP(H20,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20" t="str">
+        <f>VLOOKUP(H20,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>cancer</v>
+      </c>
+      <c r="J20" t="s">
+        <v>614</v>
+      </c>
+      <c r="K20" t="str">
+        <f>IF(J20="es","  "&amp;I20&amp;"_"&amp;J20&amp;"="&amp;VLOOKUP(I20&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J20="en","  "&amp;I20&amp;"_"&amp;J20&amp;"="&amp;VLOOKUP(I20&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J20="indice",$K$2&amp;"["&amp;H20&amp;"]",IF(J20="pnl","  pnl="&amp;G20,"  num="&amp;F20))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="3"/>
+        <v>7184</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="4"/>
+        <v>310224</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 8; 7184; 310224</v>
+      </c>
+      <c r="G21" t="str">
+        <f>VLOOKUP(H21,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21" t="str">
+        <f>VLOOKUP(H21,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>cancer</v>
+      </c>
+      <c r="J21" t="s">
         <v>126</v>
       </c>
-      <c r="D12" t="str">
-        <f>IF(C12="es","  "&amp;B12&amp;"_"&amp;C12&amp;"="&amp;VLOOKUP(B12&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C12="en","  "&amp;B12&amp;"_"&amp;C12&amp;"="&amp;VLOOKUP(B12&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A12&amp;"]"))</f>
+      <c r="K21" t="str">
+        <f>IF(J21="es","  "&amp;I21&amp;"_"&amp;J21&amp;"="&amp;VLOOKUP(I21&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J21="en","  "&amp;I21&amp;"_"&amp;J21&amp;"="&amp;VLOOKUP(I21&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J21="indice",$K$2&amp;"["&amp;H21&amp;"]",IF(J21="pnl","  pnl="&amp;G21,"  num="&amp;F21))))</f>
         <v xml:space="preserve">  cancer_es=Espera cambios sumamente positivos en lo tocante al trabajo te encontrarás en una situación laboral nueva cada vez más satisfactoria. Este es uno de esos momentos. Son buenas las condiciones para un riesgo bajo inversiones a largo plazo, ventas de propiedades y herencias. No te lances con la primera persona que se atraviese en tu camino solo porque necesites afecto o atención. Hacer ejercicio le da muchísima pereza, pero ¿tiene idea de lo que le va a alegrar ser capaz de hacer tantos abdominales? Fuera la pereza y a rejuvenecer su salud.</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="B13" t="str">
-        <f>VLOOKUP(A13,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="B22">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="3"/>
+        <v>4192</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="4"/>
+        <v>824453</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,6 y 9; 4192; 824453</v>
+      </c>
+      <c r="G22" t="str">
+        <f>VLOOKUP(H22,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22" t="str">
+        <f>VLOOKUP(H22,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>cancer</v>
       </c>
-      <c r="C13" t="s">
+      <c r="J22" t="s">
         <v>432</v>
       </c>
-      <c r="D13" t="str">
-        <f>IF(C13="es","  "&amp;B13&amp;"_"&amp;C13&amp;"="&amp;VLOOKUP(B13&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C13="en","  "&amp;B13&amp;"_"&amp;C13&amp;"="&amp;VLOOKUP(B13&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A13&amp;"]"))</f>
+      <c r="K22" t="str">
+        <f>IF(J22="es","  "&amp;I22&amp;"_"&amp;J22&amp;"="&amp;VLOOKUP(I22&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J22="en","  "&amp;I22&amp;"_"&amp;J22&amp;"="&amp;VLOOKUP(I22&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J22="indice",$K$2&amp;"["&amp;H22&amp;"]",IF(J22="pnl","  pnl="&amp;G22,"  num="&amp;F22))))</f>
         <v xml:space="preserve">  cancer_en=Expect very positive changes with regard to work you will find yourself in a new work situation more and more satisfactory. this is one of those moments. The conditions for a risk under long-term investments, property sales and inheritances are good. Do not throw yourself with the first person who crosses your path just because you need affection or attention. Exercising gives him a lot of laziness, but do you have any idea what will make him happy to be able to do so many abs? Out of laziness and to rejuvenate your health.</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="3"/>
+        <v>5244</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="4"/>
+        <v>738783</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 8; 5244; 738783</v>
+      </c>
+      <c r="G23" t="str">
+        <f>VLOOKUP(H23,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H23">
         <v>4</v>
       </c>
-      <c r="B14" t="str">
-        <f>VLOOKUP(A14,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I23" t="str">
+        <f>VLOOKUP(H23,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>leo</v>
       </c>
-      <c r="C14" t="s">
+      <c r="J23" t="s">
         <v>433</v>
       </c>
-      <c r="D14" t="str">
-        <f>IF(C14="es","  "&amp;B14&amp;"_"&amp;C14&amp;"="&amp;VLOOKUP(B14&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C14="en","  "&amp;B14&amp;"_"&amp;C14&amp;"="&amp;VLOOKUP(B14&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A14&amp;"]"))</f>
+      <c r="K23" t="str">
+        <f>IF(J23="es","  "&amp;I23&amp;"_"&amp;J23&amp;"="&amp;VLOOKUP(I23&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J23="en","  "&amp;I23&amp;"_"&amp;J23&amp;"="&amp;VLOOKUP(I23&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J23="indice",$K$2&amp;"["&amp;H23&amp;"]",IF(J23="pnl","  pnl="&amp;G23,"  num="&amp;F23))))</f>
         <v>horoscopo[4]</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="3"/>
+        <v>8006</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="4"/>
+        <v>566884</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,5 y 9; 8006; 566884</v>
+      </c>
+      <c r="G24" t="str">
+        <f>VLOOKUP(H24,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H24">
         <v>4</v>
       </c>
-      <c r="B15" t="str">
-        <f>VLOOKUP(A15,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I24" t="str">
+        <f>VLOOKUP(H24,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>leo</v>
       </c>
-      <c r="C15" t="s">
+      <c r="J24" t="s">
+        <v>613</v>
+      </c>
+      <c r="K24" t="str">
+        <f ca="1">IF(J24="es","  "&amp;I24&amp;"_"&amp;J24&amp;"="&amp;VLOOKUP(I24&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J24="en","  "&amp;I24&amp;"_"&amp;J24&amp;"="&amp;VLOOKUP(I24&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J24="indice",$K$2&amp;"["&amp;H24&amp;"]",IF(J24="pnl","  pnl="&amp;G24,"  num="&amp;F24))))</f>
+        <v xml:space="preserve">  num=1,5 y 9; 8006; 566884</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="3"/>
+        <v>2343</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="4"/>
+        <v>678368</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,5 y 8; 2343; 678368</v>
+      </c>
+      <c r="G25" t="str">
+        <f>VLOOKUP(H25,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25" t="str">
+        <f>VLOOKUP(H25,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>leo</v>
+      </c>
+      <c r="J25" t="s">
+        <v>614</v>
+      </c>
+      <c r="K25" t="str">
+        <f>IF(J25="es","  "&amp;I25&amp;"_"&amp;J25&amp;"="&amp;VLOOKUP(I25&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J25="en","  "&amp;I25&amp;"_"&amp;J25&amp;"="&amp;VLOOKUP(I25&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J25="indice",$K$2&amp;"["&amp;H25&amp;"]",IF(J25="pnl","  pnl="&amp;G25,"  num="&amp;F25))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="3"/>
+        <v>9761</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ca="1" si="4"/>
+        <v>483497</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,6 y 9; 9761; 483497</v>
+      </c>
+      <c r="G26" t="str">
+        <f>VLOOKUP(H26,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26" t="str">
+        <f>VLOOKUP(H26,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>leo</v>
+      </c>
+      <c r="J26" t="s">
         <v>126</v>
       </c>
-      <c r="D15" t="str">
-        <f>IF(C15="es","  "&amp;B15&amp;"_"&amp;C15&amp;"="&amp;VLOOKUP(B15&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C15="en","  "&amp;B15&amp;"_"&amp;C15&amp;"="&amp;VLOOKUP(B15&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A15&amp;"]"))</f>
+      <c r="K26" t="str">
+        <f>IF(J26="es","  "&amp;I26&amp;"_"&amp;J26&amp;"="&amp;VLOOKUP(I26&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J26="en","  "&amp;I26&amp;"_"&amp;J26&amp;"="&amp;VLOOKUP(I26&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J26="indice",$K$2&amp;"["&amp;H26&amp;"]",IF(J26="pnl","  pnl="&amp;G26,"  num="&amp;F26))))</f>
         <v xml:space="preserve">  leo_es=Hay competencia en el trabajo un superior está jugando el juego de un rival tuyo. ese intento de provocación puede ser una oferta de amor disfrazada. Muéstrate firme y establece claramente que no estás dispuesto a soportarlo de brazos cruzados. Es una especie de carrera contra el tiempo ahora entonces cuando alguien te pida ayuda se la negarás. La acción por impulso está excluída hoy te colocará en una posición incomoda.</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="3"/>
+        <v>3664</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="4"/>
+        <v>364313</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,7 y 8; 3664; 364313</v>
+      </c>
+      <c r="G27" t="str">
+        <f>VLOOKUP(H27,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H27">
         <v>4</v>
       </c>
-      <c r="B16" t="str">
-        <f>VLOOKUP(A16,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I27" t="str">
+        <f>VLOOKUP(H27,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>leo</v>
       </c>
-      <c r="C16" t="s">
+      <c r="J27" t="s">
         <v>432</v>
       </c>
-      <c r="D16" t="str">
-        <f>IF(C16="es","  "&amp;B16&amp;"_"&amp;C16&amp;"="&amp;VLOOKUP(B16&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C16="en","  "&amp;B16&amp;"_"&amp;C16&amp;"="&amp;VLOOKUP(B16&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A16&amp;"]"))</f>
+      <c r="K27" t="str">
+        <f>IF(J27="es","  "&amp;I27&amp;"_"&amp;J27&amp;"="&amp;VLOOKUP(I27&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J27="en","  "&amp;I27&amp;"_"&amp;J27&amp;"="&amp;VLOOKUP(I27&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J27="indice",$K$2&amp;"["&amp;H27&amp;"]",IF(J27="pnl","  pnl="&amp;G27,"  num="&amp;F27))))</f>
         <v xml:space="preserve">  leo_en=There is competition at work a superior is playing the game of a rival of yours. that attempt at provocation can be an offer of love in disguise. Be firm and clearly state that you are not willing to stand with folded arms. It is a kind of race against time now when someone asks you for help you will deny it. The action by impulse is excluded today will place you in an uncomfortable position.</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ca="1" si="3"/>
+        <v>1390</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ca="1" si="4"/>
+        <v>672766</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,7 y 8; 1390; 672766</v>
+      </c>
+      <c r="G28" t="str">
+        <f>VLOOKUP(H28,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H28">
         <v>5</v>
       </c>
-      <c r="B17" t="str">
-        <f>VLOOKUP(A17,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I28" t="str">
+        <f>VLOOKUP(H28,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>virgo</v>
       </c>
-      <c r="C17" t="s">
+      <c r="J28" t="s">
         <v>433</v>
       </c>
-      <c r="D17" t="str">
-        <f>IF(C17="es","  "&amp;B17&amp;"_"&amp;C17&amp;"="&amp;VLOOKUP(B17&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C17="en","  "&amp;B17&amp;"_"&amp;C17&amp;"="&amp;VLOOKUP(B17&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A17&amp;"]"))</f>
+      <c r="K28" t="str">
+        <f>IF(J28="es","  "&amp;I28&amp;"_"&amp;J28&amp;"="&amp;VLOOKUP(I28&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J28="en","  "&amp;I28&amp;"_"&amp;J28&amp;"="&amp;VLOOKUP(I28&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J28="indice",$K$2&amp;"["&amp;H28&amp;"]",IF(J28="pnl","  pnl="&amp;G28,"  num="&amp;F28))))</f>
         <v>horoscopo[5]</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ca="1" si="3"/>
+        <v>1335</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ca="1" si="4"/>
+        <v>393834</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,6 y 8; 1335; 393834</v>
+      </c>
+      <c r="G29" t="str">
+        <f>VLOOKUP(H29,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H29">
         <v>5</v>
       </c>
-      <c r="B18" t="str">
-        <f>VLOOKUP(A18,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I29" t="str">
+        <f>VLOOKUP(H29,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>virgo</v>
       </c>
-      <c r="C18" t="s">
+      <c r="J29" t="s">
+        <v>613</v>
+      </c>
+      <c r="K29" t="str">
+        <f ca="1">IF(J29="es","  "&amp;I29&amp;"_"&amp;J29&amp;"="&amp;VLOOKUP(I29&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J29="en","  "&amp;I29&amp;"_"&amp;J29&amp;"="&amp;VLOOKUP(I29&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J29="indice",$K$2&amp;"["&amp;H29&amp;"]",IF(J29="pnl","  pnl="&amp;G29,"  num="&amp;F29))))</f>
+        <v xml:space="preserve">  num=4,6 y 8; 1335; 393834</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="3"/>
+        <v>4976</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ca="1" si="4"/>
+        <v>216430</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,7 y 9; 4976; 216430</v>
+      </c>
+      <c r="G30" t="str">
+        <f>VLOOKUP(H30,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30" t="str">
+        <f>VLOOKUP(H30,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>virgo</v>
+      </c>
+      <c r="J30" t="s">
+        <v>614</v>
+      </c>
+      <c r="K30" t="str">
+        <f>IF(J30="es","  "&amp;I30&amp;"_"&amp;J30&amp;"="&amp;VLOOKUP(I30&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J30="en","  "&amp;I30&amp;"_"&amp;J30&amp;"="&amp;VLOOKUP(I30&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J30="indice",$K$2&amp;"["&amp;H30&amp;"]",IF(J30="pnl","  pnl="&amp;G30,"  num="&amp;F30))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ca="1" si="3"/>
+        <v>6861</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ca="1" si="4"/>
+        <v>325313</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,5 y 9; 6861; 325313</v>
+      </c>
+      <c r="G31" t="str">
+        <f>VLOOKUP(H31,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31" t="str">
+        <f>VLOOKUP(H31,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>virgo</v>
+      </c>
+      <c r="J31" t="s">
         <v>126</v>
       </c>
-      <c r="D18" t="str">
-        <f>IF(C18="es","  "&amp;B18&amp;"_"&amp;C18&amp;"="&amp;VLOOKUP(B18&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C18="en","  "&amp;B18&amp;"_"&amp;C18&amp;"="&amp;VLOOKUP(B18&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A18&amp;"]"))</f>
+      <c r="K31" t="str">
+        <f>IF(J31="es","  "&amp;I31&amp;"_"&amp;J31&amp;"="&amp;VLOOKUP(I31&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J31="en","  "&amp;I31&amp;"_"&amp;J31&amp;"="&amp;VLOOKUP(I31&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J31="indice",$K$2&amp;"["&amp;H31&amp;"]",IF(J31="pnl","  pnl="&amp;G31,"  num="&amp;F31))))</f>
         <v xml:space="preserve">  virgo_es=Vigila de cerca tus finanzas. Puedes llegar a conflicto con alguien que puede interrumpirte tu progreso al menos por el momento. Hay síntomas seguros de que estas quemando etapas En un minuto aprendes nuevas trampas y en el otro se las estás enseñando a otros. Los asuntos profesionales se presentan cargados, incluso agobiantes debes sacarlos adelante en la medida de tus posibilidades. Créelo o no pese a tu esp+irita independiente mejor unes fuerzas con alguien por razones profesionales.</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ca="1" si="3"/>
+        <v>5103</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ca="1" si="4"/>
+        <v>856290</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,6 y 8; 5103; 856290</v>
+      </c>
+      <c r="G32" t="str">
+        <f>VLOOKUP(H32,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H32">
         <v>5</v>
       </c>
-      <c r="B19" t="str">
-        <f>VLOOKUP(A19,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I32" t="str">
+        <f>VLOOKUP(H32,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>virgo</v>
       </c>
-      <c r="C19" t="s">
+      <c r="J32" t="s">
         <v>432</v>
       </c>
-      <c r="D19" t="str">
-        <f>IF(C19="es","  "&amp;B19&amp;"_"&amp;C19&amp;"="&amp;VLOOKUP(B19&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C19="en","  "&amp;B19&amp;"_"&amp;C19&amp;"="&amp;VLOOKUP(B19&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A19&amp;"]"))</f>
+      <c r="K32" t="str">
+        <f>IF(J32="es","  "&amp;I32&amp;"_"&amp;J32&amp;"="&amp;VLOOKUP(I32&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J32="en","  "&amp;I32&amp;"_"&amp;J32&amp;"="&amp;VLOOKUP(I32&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J32="indice",$K$2&amp;"["&amp;H32&amp;"]",IF(J32="pnl","  pnl="&amp;G32,"  num="&amp;F32))))</f>
         <v xml:space="preserve">  virgo_en=Keep a close eye on your finances. You can come into conflict with someone who can interrupt your progress at least for the time being. There are sure symptoms that you are burning stages In one minute you learn new traps and in the other you are teaching them to others. Professional matters are charged, even overwhelming, you must take them forward to the best of your ability. Believe it or not despite your esp + irita independent you better join forces with someone for professional reasons.</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="B20" t="str">
-        <f>VLOOKUP(A20,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="C33">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ca="1" si="3"/>
+        <v>4539</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ca="1" si="4"/>
+        <v>688969</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,6 y 9; 4539; 688969</v>
+      </c>
+      <c r="G33" t="str">
+        <f>VLOOKUP(H33,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H33">
+        <v>6</v>
+      </c>
+      <c r="I33" t="str">
+        <f>VLOOKUP(H33,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>libra</v>
       </c>
-      <c r="C20" t="s">
+      <c r="J33" t="s">
         <v>433</v>
       </c>
-      <c r="D20" t="str">
-        <f>IF(C20="es","  "&amp;B20&amp;"_"&amp;C20&amp;"="&amp;VLOOKUP(B20&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C20="en","  "&amp;B20&amp;"_"&amp;C20&amp;"="&amp;VLOOKUP(B20&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A20&amp;"]"))</f>
+      <c r="K33" t="str">
+        <f>IF(J33="es","  "&amp;I33&amp;"_"&amp;J33&amp;"="&amp;VLOOKUP(I33&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J33="en","  "&amp;I33&amp;"_"&amp;J33&amp;"="&amp;VLOOKUP(I33&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J33="indice",$K$2&amp;"["&amp;H33&amp;"]",IF(J33="pnl","  pnl="&amp;G33,"  num="&amp;F33))))</f>
         <v>horoscopo[6]</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ca="1" si="3"/>
+        <v>4483</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ca="1" si="4"/>
+        <v>450557</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,7 y 9; 4483; 450557</v>
+      </c>
+      <c r="G34" t="str">
+        <f>VLOOKUP(H34,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H34">
         <v>6</v>
       </c>
-      <c r="B21" t="str">
-        <f>VLOOKUP(A21,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I34" t="str">
+        <f>VLOOKUP(H34,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>libra</v>
       </c>
-      <c r="C21" t="s">
+      <c r="J34" t="s">
+        <v>613</v>
+      </c>
+      <c r="K34" t="str">
+        <f ca="1">IF(J34="es","  "&amp;I34&amp;"_"&amp;J34&amp;"="&amp;VLOOKUP(I34&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J34="en","  "&amp;I34&amp;"_"&amp;J34&amp;"="&amp;VLOOKUP(I34&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J34="indice",$K$2&amp;"["&amp;H34&amp;"]",IF(J34="pnl","  pnl="&amp;G34,"  num="&amp;F34))))</f>
+        <v xml:space="preserve">  num=1,7 y 9; 4483; 450557</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ca="1" si="3"/>
+        <v>8808</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ca="1" si="4"/>
+        <v>106597</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,6 y 8; 8808; 106597</v>
+      </c>
+      <c r="G35" t="str">
+        <f>VLOOKUP(H35,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H35">
+        <v>6</v>
+      </c>
+      <c r="I35" t="str">
+        <f>VLOOKUP(H35,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>libra</v>
+      </c>
+      <c r="J35" t="s">
+        <v>614</v>
+      </c>
+      <c r="K35" t="str">
+        <f>IF(J35="es","  "&amp;I35&amp;"_"&amp;J35&amp;"="&amp;VLOOKUP(I35&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J35="en","  "&amp;I35&amp;"_"&amp;J35&amp;"="&amp;VLOOKUP(I35&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J35="indice",$K$2&amp;"["&amp;H35&amp;"]",IF(J35="pnl","  pnl="&amp;G35,"  num="&amp;F35))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ca="1" si="3"/>
+        <v>9027</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ca="1" si="4"/>
+        <v>426452</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,5 y 9; 9027; 426452</v>
+      </c>
+      <c r="G36" t="str">
+        <f>VLOOKUP(H36,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36" t="str">
+        <f>VLOOKUP(H36,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>libra</v>
+      </c>
+      <c r="J36" t="s">
         <v>126</v>
       </c>
-      <c r="D21" t="str">
-        <f>IF(C21="es","  "&amp;B21&amp;"_"&amp;C21&amp;"="&amp;VLOOKUP(B21&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C21="en","  "&amp;B21&amp;"_"&amp;C21&amp;"="&amp;VLOOKUP(B21&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A21&amp;"]"))</f>
+      <c r="K36" t="str">
+        <f>IF(J36="es","  "&amp;I36&amp;"_"&amp;J36&amp;"="&amp;VLOOKUP(I36&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J36="en","  "&amp;I36&amp;"_"&amp;J36&amp;"="&amp;VLOOKUP(I36&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J36="indice",$K$2&amp;"["&amp;H36&amp;"]",IF(J36="pnl","  pnl="&amp;G36,"  num="&amp;F36))))</f>
         <v xml:space="preserve">  libra_es=Hay grandes cambios en puerta para tí en todos los aspectos en los próximos meses estás fuertemente avisado para que lo tomes con calma y te prepares para tiempos difíciles. El la vida hay algo mas que sòlo trabajo, trabajo y trabajo Algo ocurre hoy que te recuerda que es hora de espabilarte y gozar de la vida. Los viajes, la carrera y las finanzas están íntimamente vinculados puede ser que se presente una oportunidad en la carrera. Las finanzas juegan un creciente papel en tu actual línea de pensamiento Toma ventaja de la situación y mira a ver cómo puedes mejorar tu seguridad a largo plazo. Hoy es un día para recuperar recuerdos.</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="B22" t="str">
-        <f>VLOOKUP(A22,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="C37">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ca="1" si="3"/>
+        <v>7173</v>
+      </c>
+      <c r="E37">
+        <f t="shared" ca="1" si="4"/>
+        <v>662035</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 9; 7173; 662035</v>
+      </c>
+      <c r="G37" t="str">
+        <f>VLOOKUP(H37,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H37">
+        <v>6</v>
+      </c>
+      <c r="I37" t="str">
+        <f>VLOOKUP(H37,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>libra</v>
       </c>
-      <c r="C22" t="s">
+      <c r="J37" t="s">
         <v>432</v>
       </c>
-      <c r="D22" t="str">
-        <f>IF(C22="es","  "&amp;B22&amp;"_"&amp;C22&amp;"="&amp;VLOOKUP(B22&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C22="en","  "&amp;B22&amp;"_"&amp;C22&amp;"="&amp;VLOOKUP(B22&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A22&amp;"]"))</f>
+      <c r="K37" t="str">
+        <f>IF(J37="es","  "&amp;I37&amp;"_"&amp;J37&amp;"="&amp;VLOOKUP(I37&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J37="en","  "&amp;I37&amp;"_"&amp;J37&amp;"="&amp;VLOOKUP(I37&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J37="indice",$K$2&amp;"["&amp;H37&amp;"]",IF(J37="pnl","  pnl="&amp;G37,"  num="&amp;F37))))</f>
         <v xml:space="preserve">  libra_en=Hay grandes cambios en puerta para tí en todos los aspectos en los próximos meses estás fuertemente avisado para que lo tomes con calma y te prepares para tiempos difíciles. El la vida hay algo mas que sòlo trabajo, trabajo y trabajo Algo ocurre hoy que te recuerda que es hora de espabilarte y gozar de la vida. Los viajes, la carrera y las finanzas están íntimamente vinculados puede ser que se presente una oportunidad en la carrera. Las finanzas juegan un creciente papel en tu actual línea de pensamiento Toma ventaja de la situación y mira a ver cómo puedes mejorar tu seguridad a largo plazo. Hoy es un día para recuperar recuerdos.</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ca="1" si="3"/>
+        <v>7866</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ca="1" si="4"/>
+        <v>482905</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,5 y 8; 7866; 482905</v>
+      </c>
+      <c r="G38" t="str">
+        <f>VLOOKUP(H38,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H38">
         <v>7</v>
       </c>
-      <c r="B23" t="str">
-        <f>VLOOKUP(A23,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I38" t="str">
+        <f>VLOOKUP(H38,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>escorpio</v>
       </c>
-      <c r="C23" t="s">
+      <c r="J38" t="s">
         <v>433</v>
       </c>
-      <c r="D23" t="str">
-        <f>IF(C23="es","  "&amp;B23&amp;"_"&amp;C23&amp;"="&amp;VLOOKUP(B23&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C23="en","  "&amp;B23&amp;"_"&amp;C23&amp;"="&amp;VLOOKUP(B23&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A23&amp;"]"))</f>
+      <c r="K38" t="str">
+        <f>IF(J38="es","  "&amp;I38&amp;"_"&amp;J38&amp;"="&amp;VLOOKUP(I38&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J38="en","  "&amp;I38&amp;"_"&amp;J38&amp;"="&amp;VLOOKUP(I38&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J38="indice",$K$2&amp;"["&amp;H38&amp;"]",IF(J38="pnl","  pnl="&amp;G38,"  num="&amp;F38))))</f>
         <v>horoscopo[7]</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ca="1" si="3"/>
+        <v>4386</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ca="1" si="4"/>
+        <v>458065</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,6 y 8; 4386; 458065</v>
+      </c>
+      <c r="G39" t="str">
+        <f>VLOOKUP(H39,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H39">
         <v>7</v>
       </c>
-      <c r="B24" t="str">
-        <f>VLOOKUP(A24,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I39" t="str">
+        <f>VLOOKUP(H39,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>escorpio</v>
       </c>
-      <c r="C24" t="s">
+      <c r="J39" t="s">
+        <v>613</v>
+      </c>
+      <c r="K39" t="str">
+        <f ca="1">IF(J39="es","  "&amp;I39&amp;"_"&amp;J39&amp;"="&amp;VLOOKUP(I39&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J39="en","  "&amp;I39&amp;"_"&amp;J39&amp;"="&amp;VLOOKUP(I39&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J39="indice",$K$2&amp;"["&amp;H39&amp;"]",IF(J39="pnl","  pnl="&amp;G39,"  num="&amp;F39))))</f>
+        <v xml:space="preserve">  num=4,6 y 8; 4386; 458065</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ca="1" si="3"/>
+        <v>4819</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ca="1" si="4"/>
+        <v>671878</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,7 y 8; 4819; 671878</v>
+      </c>
+      <c r="G40" t="str">
+        <f>VLOOKUP(H40,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H40">
+        <v>7</v>
+      </c>
+      <c r="I40" t="str">
+        <f>VLOOKUP(H40,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>escorpio</v>
+      </c>
+      <c r="J40" t="s">
+        <v>614</v>
+      </c>
+      <c r="K40" t="str">
+        <f>IF(J40="es","  "&amp;I40&amp;"_"&amp;J40&amp;"="&amp;VLOOKUP(I40&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J40="en","  "&amp;I40&amp;"_"&amp;J40&amp;"="&amp;VLOOKUP(I40&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J40="indice",$K$2&amp;"["&amp;H40&amp;"]",IF(J40="pnl","  pnl="&amp;G40,"  num="&amp;F40))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ca="1" si="3"/>
+        <v>6651</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ca="1" si="4"/>
+        <v>379262</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 9; 6651; 379262</v>
+      </c>
+      <c r="G41" t="str">
+        <f>VLOOKUP(H41,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+      <c r="I41" t="str">
+        <f>VLOOKUP(H41,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>escorpio</v>
+      </c>
+      <c r="J41" t="s">
         <v>126</v>
       </c>
-      <c r="D24" t="str">
-        <f>IF(C24="es","  "&amp;B24&amp;"_"&amp;C24&amp;"="&amp;VLOOKUP(B24&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C24="en","  "&amp;B24&amp;"_"&amp;C24&amp;"="&amp;VLOOKUP(B24&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A24&amp;"]"))</f>
+      <c r="K41" t="str">
+        <f>IF(J41="es","  "&amp;I41&amp;"_"&amp;J41&amp;"="&amp;VLOOKUP(I41&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J41="en","  "&amp;I41&amp;"_"&amp;J41&amp;"="&amp;VLOOKUP(I41&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J41="indice",$K$2&amp;"["&amp;H41&amp;"]",IF(J41="pnl","  pnl="&amp;G41,"  num="&amp;F41))))</f>
         <v xml:space="preserve">  escorpio_es=Estás en disposición de admitir que has cometido un error No tienes que publicarlo. Otros harán que las cosas se vean a su manera No vas a empecinarte pero sí a mantener tus posiciones. Con sólo desear, esperar y soñar no es suficiente para ir a donde deseas Toma una acción concreta. Las decisiones financieras hechas el día de hoy pueden resultar ser una excelente inversión para el futuro. Si te apetece, adelante, no lo pienses.</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ca="1" si="3"/>
+        <v>1625</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ca="1" si="4"/>
+        <v>105799</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 8; 1625; 105799</v>
+      </c>
+      <c r="G42" t="str">
+        <f>VLOOKUP(H42,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H42">
         <v>7</v>
       </c>
-      <c r="B25" t="str">
-        <f>VLOOKUP(A25,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I42" t="str">
+        <f>VLOOKUP(H42,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>escorpio</v>
       </c>
-      <c r="C25" t="s">
+      <c r="J42" t="s">
         <v>432</v>
       </c>
-      <c r="D25" t="str">
-        <f>IF(C25="es","  "&amp;B25&amp;"_"&amp;C25&amp;"="&amp;VLOOKUP(B25&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C25="en","  "&amp;B25&amp;"_"&amp;C25&amp;"="&amp;VLOOKUP(B25&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A25&amp;"]"))</f>
+      <c r="K42" t="str">
+        <f>IF(J42="es","  "&amp;I42&amp;"_"&amp;J42&amp;"="&amp;VLOOKUP(I42&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J42="en","  "&amp;I42&amp;"_"&amp;J42&amp;"="&amp;VLOOKUP(I42&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J42="indice",$K$2&amp;"["&amp;H42&amp;"]",IF(J42="pnl","  pnl="&amp;G42,"  num="&amp;F42))))</f>
         <v xml:space="preserve">  escorpio_en=You are willing to admit that you have made a mistake. You do not have to publish it. Others will make things look their way You will not stubbornly but you will keep your positions. Just wanting, waiting and dreaming is not enough to go where you want Take a concrete action. Financial decisions made today can prove to be an excellent investment for the future. If you feel like it, go ahead, do not think about it.</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ca="1" si="3"/>
+        <v>7544</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ca="1" si="4"/>
+        <v>726750</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 9; 7544; 726750</v>
+      </c>
+      <c r="G43" t="str">
+        <f>VLOOKUP(H43,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H43">
         <v>8</v>
       </c>
-      <c r="B26" t="str">
-        <f>VLOOKUP(A26,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I43" t="str">
+        <f>VLOOKUP(H43,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>sagitario</v>
       </c>
-      <c r="C26" t="s">
+      <c r="J43" t="s">
         <v>433</v>
       </c>
-      <c r="D26" t="str">
-        <f>IF(C26="es","  "&amp;B26&amp;"_"&amp;C26&amp;"="&amp;VLOOKUP(B26&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C26="en","  "&amp;B26&amp;"_"&amp;C26&amp;"="&amp;VLOOKUP(B26&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A26&amp;"]"))</f>
+      <c r="K43" t="str">
+        <f>IF(J43="es","  "&amp;I43&amp;"_"&amp;J43&amp;"="&amp;VLOOKUP(I43&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J43="en","  "&amp;I43&amp;"_"&amp;J43&amp;"="&amp;VLOOKUP(I43&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J43="indice",$K$2&amp;"["&amp;H43&amp;"]",IF(J43="pnl","  pnl="&amp;G43,"  num="&amp;F43))))</f>
         <v>horoscopo[8]</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ca="1" si="3"/>
+        <v>2293</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ca="1" si="4"/>
+        <v>190951</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 9; 2293; 190951</v>
+      </c>
+      <c r="G44" t="str">
+        <f>VLOOKUP(H44,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H44">
         <v>8</v>
       </c>
-      <c r="B27" t="str">
-        <f>VLOOKUP(A27,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I44" t="str">
+        <f>VLOOKUP(H44,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>sagitario</v>
       </c>
-      <c r="C27" t="s">
+      <c r="J44" t="s">
+        <v>613</v>
+      </c>
+      <c r="K44" t="str">
+        <f ca="1">IF(J44="es","  "&amp;I44&amp;"_"&amp;J44&amp;"="&amp;VLOOKUP(I44&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J44="en","  "&amp;I44&amp;"_"&amp;J44&amp;"="&amp;VLOOKUP(I44&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J44="indice",$K$2&amp;"["&amp;H44&amp;"]",IF(J44="pnl","  pnl="&amp;G44,"  num="&amp;F44))))</f>
+        <v xml:space="preserve">  num=1,6 y 9; 2293; 190951</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ca="1" si="3"/>
+        <v>5784</v>
+      </c>
+      <c r="E45">
+        <f t="shared" ca="1" si="4"/>
+        <v>512159</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,6 y 9; 5784; 512159</v>
+      </c>
+      <c r="G45" t="str">
+        <f>VLOOKUP(H45,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45" t="str">
+        <f>VLOOKUP(H45,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>sagitario</v>
+      </c>
+      <c r="J45" t="s">
+        <v>614</v>
+      </c>
+      <c r="K45" t="str">
+        <f>IF(J45="es","  "&amp;I45&amp;"_"&amp;J45&amp;"="&amp;VLOOKUP(I45&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J45="en","  "&amp;I45&amp;"_"&amp;J45&amp;"="&amp;VLOOKUP(I45&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J45="indice",$K$2&amp;"["&amp;H45&amp;"]",IF(J45="pnl","  pnl="&amp;G45,"  num="&amp;F45))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ca="1" si="3"/>
+        <v>6428</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ca="1" si="4"/>
+        <v>697745</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,6 y 8; 6428; 697745</v>
+      </c>
+      <c r="G46" t="str">
+        <f>VLOOKUP(H46,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H46">
+        <v>8</v>
+      </c>
+      <c r="I46" t="str">
+        <f>VLOOKUP(H46,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>sagitario</v>
+      </c>
+      <c r="J46" t="s">
         <v>126</v>
       </c>
-      <c r="D27" t="str">
-        <f>IF(C27="es","  "&amp;B27&amp;"_"&amp;C27&amp;"="&amp;VLOOKUP(B27&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C27="en","  "&amp;B27&amp;"_"&amp;C27&amp;"="&amp;VLOOKUP(B27&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A27&amp;"]"))</f>
+      <c r="K46" t="str">
+        <f>IF(J46="es","  "&amp;I46&amp;"_"&amp;J46&amp;"="&amp;VLOOKUP(I46&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J46="en","  "&amp;I46&amp;"_"&amp;J46&amp;"="&amp;VLOOKUP(I46&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J46="indice",$K$2&amp;"["&amp;H46&amp;"]",IF(J46="pnl","  pnl="&amp;G46,"  num="&amp;F46))))</f>
         <v xml:space="preserve">  sagitario_es=Si actúas movida por el capricho, acabarás adquiriendo algo a sobreprecio o que no vale la pena Se necesita algo de contención por lo menos en las cuestiones de dinero. Tienes una fuente infinita de coraje que te ayudará en momentos duros. Las fuerzas astrales te animan a olvidar tus obligaciones hoy puedes estimar que los compromises con tu carrera son un fardo, y tu atención se desvía con facilidad. Se puede resolver un dilema si así te lo propones aplica tus poderes de concentración y análisis. Unos encuentros agradables le devolverán la confianza en los demás</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ca="1" si="3"/>
+        <v>1812</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ca="1" si="4"/>
+        <v>743805</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,7 y 9; 1812; 743805</v>
+      </c>
+      <c r="G47" t="str">
+        <f>VLOOKUP(H47,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H47">
         <v>8</v>
       </c>
-      <c r="B28" t="str">
-        <f>VLOOKUP(A28,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I47" t="str">
+        <f>VLOOKUP(H47,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>sagitario</v>
       </c>
-      <c r="C28" t="s">
+      <c r="J47" t="s">
         <v>432</v>
       </c>
-      <c r="D28" t="str">
-        <f>IF(C28="es","  "&amp;B28&amp;"_"&amp;C28&amp;"="&amp;VLOOKUP(B28&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C28="en","  "&amp;B28&amp;"_"&amp;C28&amp;"="&amp;VLOOKUP(B28&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A28&amp;"]"))</f>
+      <c r="K47" t="str">
+        <f>IF(J47="es","  "&amp;I47&amp;"_"&amp;J47&amp;"="&amp;VLOOKUP(I47&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J47="en","  "&amp;I47&amp;"_"&amp;J47&amp;"="&amp;VLOOKUP(I47&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J47="indice",$K$2&amp;"["&amp;H47&amp;"]",IF(J47="pnl","  pnl="&amp;G47,"  num="&amp;F47))))</f>
         <v xml:space="preserve">  sagitario_en=If you act on a whim, you will end up acquiring something at a premium or that it is not worth it. Some restraint is needed, at least in matters of money. You have an infinite source of courage that will help you in hard times. The astral forces encourage you to forget your obligations today you can estimate that the compromises with your career are a burden, and your attention deviates easily. A dilemma can be resolved if you propose to apply your powers of concentration and analysis. Pleasant encounters will restore confidence in others</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="B29" t="str">
-        <f>VLOOKUP(A29,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="D48">
+        <f t="shared" ca="1" si="3"/>
+        <v>4411</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ca="1" si="4"/>
+        <v>901729</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,5 y 9; 4411; 901729</v>
+      </c>
+      <c r="G48" t="str">
+        <f>VLOOKUP(H48,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H48">
+        <v>9</v>
+      </c>
+      <c r="I48" t="str">
+        <f>VLOOKUP(H48,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>capricornio</v>
       </c>
-      <c r="C29" t="s">
+      <c r="J48" t="s">
         <v>433</v>
       </c>
-      <c r="D29" t="str">
-        <f>IF(C29="es","  "&amp;B29&amp;"_"&amp;C29&amp;"="&amp;VLOOKUP(B29&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C29="en","  "&amp;B29&amp;"_"&amp;C29&amp;"="&amp;VLOOKUP(B29&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A29&amp;"]"))</f>
+      <c r="K48" t="str">
+        <f>IF(J48="es","  "&amp;I48&amp;"_"&amp;J48&amp;"="&amp;VLOOKUP(I48&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J48="en","  "&amp;I48&amp;"_"&amp;J48&amp;"="&amp;VLOOKUP(I48&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J48="indice",$K$2&amp;"["&amp;H48&amp;"]",IF(J48="pnl","  pnl="&amp;G48,"  num="&amp;F48))))</f>
         <v>horoscopo[9]</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="B30" t="str">
-        <f>VLOOKUP(A30,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="D49">
+        <f t="shared" ca="1" si="3"/>
+        <v>6966</v>
+      </c>
+      <c r="E49">
+        <f t="shared" ca="1" si="4"/>
+        <v>277107</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,6 y 9; 6966; 277107</v>
+      </c>
+      <c r="G49" t="str">
+        <f>VLOOKUP(H49,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H49">
+        <v>9</v>
+      </c>
+      <c r="I49" t="str">
+        <f>VLOOKUP(H49,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>capricornio</v>
       </c>
-      <c r="C30" t="s">
+      <c r="J49" t="s">
+        <v>613</v>
+      </c>
+      <c r="K49" t="str">
+        <f ca="1">IF(J49="es","  "&amp;I49&amp;"_"&amp;J49&amp;"="&amp;VLOOKUP(I49&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J49="en","  "&amp;I49&amp;"_"&amp;J49&amp;"="&amp;VLOOKUP(I49&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J49="indice",$K$2&amp;"["&amp;H49&amp;"]",IF(J49="pnl","  pnl="&amp;G49,"  num="&amp;F49))))</f>
+        <v xml:space="preserve">  num=3,6 y 9; 6966; 277107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ca="1" si="3"/>
+        <v>6033</v>
+      </c>
+      <c r="E50">
+        <f t="shared" ca="1" si="4"/>
+        <v>179074</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,5 y 9; 6033; 179074</v>
+      </c>
+      <c r="G50" t="str">
+        <f>VLOOKUP(H50,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H50">
+        <v>9</v>
+      </c>
+      <c r="I50" t="str">
+        <f>VLOOKUP(H50,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>capricornio</v>
+      </c>
+      <c r="J50" t="s">
+        <v>614</v>
+      </c>
+      <c r="K50" t="str">
+        <f>IF(J50="es","  "&amp;I50&amp;"_"&amp;J50&amp;"="&amp;VLOOKUP(I50&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J50="en","  "&amp;I50&amp;"_"&amp;J50&amp;"="&amp;VLOOKUP(I50&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J50="indice",$K$2&amp;"["&amp;H50&amp;"]",IF(J50="pnl","  pnl="&amp;G50,"  num="&amp;F50))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ca="1" si="3"/>
+        <v>6446</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ca="1" si="4"/>
+        <v>566389</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,6 y 9; 6446; 566389</v>
+      </c>
+      <c r="G51" t="str">
+        <f>VLOOKUP(H51,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H51">
+        <v>9</v>
+      </c>
+      <c r="I51" t="str">
+        <f>VLOOKUP(H51,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>capricornio</v>
+      </c>
+      <c r="J51" t="s">
         <v>126</v>
       </c>
-      <c r="D30" t="str">
-        <f>IF(C30="es","  "&amp;B30&amp;"_"&amp;C30&amp;"="&amp;VLOOKUP(B30&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C30="en","  "&amp;B30&amp;"_"&amp;C30&amp;"="&amp;VLOOKUP(B30&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A30&amp;"]"))</f>
+      <c r="K51" t="str">
+        <f>IF(J51="es","  "&amp;I51&amp;"_"&amp;J51&amp;"="&amp;VLOOKUP(I51&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J51="en","  "&amp;I51&amp;"_"&amp;J51&amp;"="&amp;VLOOKUP(I51&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J51="indice",$K$2&amp;"["&amp;H51&amp;"]",IF(J51="pnl","  pnl="&amp;G51,"  num="&amp;F51))))</f>
         <v xml:space="preserve">  capricornio_es=Estás radiante, conquistas y tu actitud vital es tan positiva y optimista que todos queremos arrimarnos a ti por si se nos pega algo de tu energía. En tu Casa cinco sacará a relucir al jugador competitivo e impetuoso que apuesta hasta la ropa interior en el terreno del amor. Esto incrementará tu popularidad hasta llegar a producir efectos que te sorprenderán. Quizá venga de la mano de un trabajo que complemente al que ya tienes. Estás tocado por la varita mágica de la palabra, así que aprovéchalo.</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="B31" t="str">
-        <f>VLOOKUP(A31,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="D52">
+        <f t="shared" ca="1" si="3"/>
+        <v>4113</v>
+      </c>
+      <c r="E52">
+        <f t="shared" ca="1" si="4"/>
+        <v>752041</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,7 y 9; 4113; 752041</v>
+      </c>
+      <c r="G52" t="str">
+        <f>VLOOKUP(H52,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H52">
+        <v>9</v>
+      </c>
+      <c r="I52" t="str">
+        <f>VLOOKUP(H52,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>capricornio</v>
       </c>
-      <c r="C31" t="s">
+      <c r="J52" t="s">
         <v>432</v>
       </c>
-      <c r="D31" t="str">
-        <f>IF(C31="es","  "&amp;B31&amp;"_"&amp;C31&amp;"="&amp;VLOOKUP(B31&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C31="en","  "&amp;B31&amp;"_"&amp;C31&amp;"="&amp;VLOOKUP(B31&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A31&amp;"]"))</f>
+      <c r="K52" t="str">
+        <f>IF(J52="es","  "&amp;I52&amp;"_"&amp;J52&amp;"="&amp;VLOOKUP(I52&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J52="en","  "&amp;I52&amp;"_"&amp;J52&amp;"="&amp;VLOOKUP(I52&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J52="indice",$K$2&amp;"["&amp;H52&amp;"]",IF(J52="pnl","  pnl="&amp;G52,"  num="&amp;F52))))</f>
         <v xml:space="preserve">  capricornio_en=You are radiant, you conquer and your vital attitude is so positive and optimistic that we all want to get close to you in case some of your energy hits us. In your House five will bring up the competitive and impetuous player who bets up underwear in the field of love. This will increase your popularity to produce effects that will surprise you. Maybe it comes from the hand of a job that complements the one you already have. You are touched by the magic wand of the word, so take advantage of it.</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ca="1" si="3"/>
+        <v>7708</v>
+      </c>
+      <c r="E53">
+        <f t="shared" ca="1" si="4"/>
+        <v>268635</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,5 y 8; 7708; 268635</v>
+      </c>
+      <c r="G53" t="str">
+        <f>VLOOKUP(H53,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H53">
         <v>10</v>
       </c>
-      <c r="B32" t="str">
-        <f>VLOOKUP(A32,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I53" t="str">
+        <f>VLOOKUP(H53,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>acuario</v>
       </c>
-      <c r="C32" t="s">
+      <c r="J53" t="s">
         <v>433</v>
       </c>
-      <c r="D32" t="str">
-        <f>IF(C32="es","  "&amp;B32&amp;"_"&amp;C32&amp;"="&amp;VLOOKUP(B32&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C32="en","  "&amp;B32&amp;"_"&amp;C32&amp;"="&amp;VLOOKUP(B32&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A32&amp;"]"))</f>
+      <c r="K53" t="str">
+        <f>IF(J53="es","  "&amp;I53&amp;"_"&amp;J53&amp;"="&amp;VLOOKUP(I53&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J53="en","  "&amp;I53&amp;"_"&amp;J53&amp;"="&amp;VLOOKUP(I53&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J53="indice",$K$2&amp;"["&amp;H53&amp;"]",IF(J53="pnl","  pnl="&amp;G53,"  num="&amp;F53))))</f>
         <v>horoscopo[10]</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ca="1" si="3"/>
+        <v>5696</v>
+      </c>
+      <c r="E54">
+        <f t="shared" ca="1" si="4"/>
+        <v>351239</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,5 y 9; 5696; 351239</v>
+      </c>
+      <c r="G54" t="str">
+        <f>VLOOKUP(H54,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H54">
         <v>10</v>
       </c>
-      <c r="B33" t="str">
-        <f>VLOOKUP(A33,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I54" t="str">
+        <f>VLOOKUP(H54,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>acuario</v>
       </c>
-      <c r="C33" t="s">
+      <c r="J54" t="s">
+        <v>613</v>
+      </c>
+      <c r="K54" t="str">
+        <f ca="1">IF(J54="es","  "&amp;I54&amp;"_"&amp;J54&amp;"="&amp;VLOOKUP(I54&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J54="en","  "&amp;I54&amp;"_"&amp;J54&amp;"="&amp;VLOOKUP(I54&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J54="indice",$K$2&amp;"["&amp;H54&amp;"]",IF(J54="pnl","  pnl="&amp;G54,"  num="&amp;F54))))</f>
+        <v xml:space="preserve">  num=3,5 y 9; 5696; 351239</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ca="1" si="3"/>
+        <v>2202</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ca="1" si="4"/>
+        <v>404306</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,7 y 8; 2202; 404306</v>
+      </c>
+      <c r="G55" t="str">
+        <f>VLOOKUP(H55,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H55">
+        <v>10</v>
+      </c>
+      <c r="I55" t="str">
+        <f>VLOOKUP(H55,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>acuario</v>
+      </c>
+      <c r="J55" t="s">
+        <v>614</v>
+      </c>
+      <c r="K55" t="str">
+        <f>IF(J55="es","  "&amp;I55&amp;"_"&amp;J55&amp;"="&amp;VLOOKUP(I55&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J55="en","  "&amp;I55&amp;"_"&amp;J55&amp;"="&amp;VLOOKUP(I55&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J55="indice",$K$2&amp;"["&amp;H55&amp;"]",IF(J55="pnl","  pnl="&amp;G55,"  num="&amp;F55))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ca="1" si="3"/>
+        <v>1385</v>
+      </c>
+      <c r="E56">
+        <f t="shared" ca="1" si="4"/>
+        <v>904022</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,5 y 9; 1385; 904022</v>
+      </c>
+      <c r="G56" t="str">
+        <f>VLOOKUP(H56,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H56">
+        <v>10</v>
+      </c>
+      <c r="I56" t="str">
+        <f>VLOOKUP(H56,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>acuario</v>
+      </c>
+      <c r="J56" t="s">
         <v>126</v>
       </c>
-      <c r="D33" t="str">
-        <f>IF(C33="es","  "&amp;B33&amp;"_"&amp;C33&amp;"="&amp;VLOOKUP(B33&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C33="en","  "&amp;B33&amp;"_"&amp;C33&amp;"="&amp;VLOOKUP(B33&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A33&amp;"]"))</f>
+      <c r="K56" t="str">
+        <f>IF(J56="es","  "&amp;I56&amp;"_"&amp;J56&amp;"="&amp;VLOOKUP(I56&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J56="en","  "&amp;I56&amp;"_"&amp;J56&amp;"="&amp;VLOOKUP(I56&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J56="indice",$K$2&amp;"["&amp;H56&amp;"]",IF(J56="pnl","  pnl="&amp;G56,"  num="&amp;F56))))</f>
         <v xml:space="preserve">  acuario_es=Quires salir adelante pero también quieres hacer feliz a otros Eso significa un duro equilibrio y la avenencia es imprescindible. Puede que otros hagan mas ruido que tú pero tu eres dueño de tu serenidad y de tu independencia. Es más fácil de lo que crees. Agradece las cosas buenas que tienes y las habrá mejores. Si los demás no le reconocen abiertamente, usted se sentirá decepcionado y asumirá la posición y los privilegios que considera que le corresponden.</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B57">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ca="1" si="3"/>
+        <v>7541</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ca="1" si="4"/>
+        <v>927148</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,7 y 9; 7541; 927148</v>
+      </c>
+      <c r="G57" t="str">
+        <f>VLOOKUP(H57,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H57">
         <v>10</v>
       </c>
-      <c r="B34" t="str">
-        <f>VLOOKUP(A34,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I57" t="str">
+        <f>VLOOKUP(H57,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>acuario</v>
       </c>
-      <c r="C34" t="s">
+      <c r="J57" t="s">
         <v>432</v>
       </c>
-      <c r="D34" t="str">
-        <f>IF(C34="es","  "&amp;B34&amp;"_"&amp;C34&amp;"="&amp;VLOOKUP(B34&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C34="en","  "&amp;B34&amp;"_"&amp;C34&amp;"="&amp;VLOOKUP(B34&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A34&amp;"]"))</f>
+      <c r="K57" t="str">
+        <f>IF(J57="es","  "&amp;I57&amp;"_"&amp;J57&amp;"="&amp;VLOOKUP(I57&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J57="en","  "&amp;I57&amp;"_"&amp;J57&amp;"="&amp;VLOOKUP(I57&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J57="indice",$K$2&amp;"["&amp;H57&amp;"]",IF(J57="pnl","  pnl="&amp;G57,"  num="&amp;F57))))</f>
         <v xml:space="preserve">  acuario_en=You want to get ahead but you also want to make others happy. That means a hard balance and compromise is essential. Others may make more noise than you but you are the owner of your serenity and independence. It is easier than you think. Thanks for the good things you have and there will be better things. If others do not openly acknowledge you, you will be disappointed and assume the position and privileges that you consider appropriate.</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ca="1" si="3"/>
+        <v>2853</v>
+      </c>
+      <c r="E58">
+        <f t="shared" ca="1" si="4"/>
+        <v>436249</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>1,7 y 8; 2853; 436249</v>
+      </c>
+      <c r="G58" t="str">
+        <f>VLOOKUP(H58,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H58">
         <v>11</v>
       </c>
-      <c r="B35" t="str">
-        <f>VLOOKUP(A35,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I58" t="str">
+        <f>VLOOKUP(H58,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>piscis</v>
       </c>
-      <c r="C35" t="s">
+      <c r="J58" t="s">
         <v>433</v>
       </c>
-      <c r="D35" t="str">
-        <f>IF(C35="es","  "&amp;B35&amp;"_"&amp;C35&amp;"="&amp;VLOOKUP(B35&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C35="en","  "&amp;B35&amp;"_"&amp;C35&amp;"="&amp;VLOOKUP(B35&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A35&amp;"]"))</f>
+      <c r="K58" t="str">
+        <f>IF(J58="es","  "&amp;I58&amp;"_"&amp;J58&amp;"="&amp;VLOOKUP(I58&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J58="en","  "&amp;I58&amp;"_"&amp;J58&amp;"="&amp;VLOOKUP(I58&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J58="indice",$K$2&amp;"["&amp;H58&amp;"]",IF(J58="pnl","  pnl="&amp;G58,"  num="&amp;F58))))</f>
         <v>horoscopo[11]</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C59">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D59">
+        <f t="shared" ca="1" si="3"/>
+        <v>4222</v>
+      </c>
+      <c r="E59">
+        <f t="shared" ca="1" si="4"/>
+        <v>868025</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>3,6 y 8; 4222; 868025</v>
+      </c>
+      <c r="G59" t="str">
+        <f>VLOOKUP(H59,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H59">
         <v>11</v>
       </c>
-      <c r="B36" t="str">
-        <f>VLOOKUP(A36,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I59" t="str">
+        <f>VLOOKUP(H59,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>piscis</v>
       </c>
-      <c r="C36" t="s">
+      <c r="J59" t="s">
+        <v>613</v>
+      </c>
+      <c r="K59" t="str">
+        <f ca="1">IF(J59="es","  "&amp;I59&amp;"_"&amp;J59&amp;"="&amp;VLOOKUP(I59&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J59="en","  "&amp;I59&amp;"_"&amp;J59&amp;"="&amp;VLOOKUP(I59&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J59="indice",$K$2&amp;"["&amp;H59&amp;"]",IF(J59="pnl","  pnl="&amp;G59,"  num="&amp;F59))))</f>
+        <v xml:space="preserve">  num=3,6 y 8; 4222; 868025</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D60">
+        <f t="shared" ca="1" si="3"/>
+        <v>4311</v>
+      </c>
+      <c r="E60">
+        <f t="shared" ca="1" si="4"/>
+        <v>536719</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,5 y 9; 4311; 536719</v>
+      </c>
+      <c r="G60" t="str">
+        <f>VLOOKUP(H60,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H60">
+        <v>11</v>
+      </c>
+      <c r="I60" t="str">
+        <f>VLOOKUP(H60,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>piscis</v>
+      </c>
+      <c r="J60" t="s">
+        <v>614</v>
+      </c>
+      <c r="K60" t="str">
+        <f>IF(J60="es","  "&amp;I60&amp;"_"&amp;J60&amp;"="&amp;VLOOKUP(I60&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J60="en","  "&amp;I60&amp;"_"&amp;J60&amp;"="&amp;VLOOKUP(I60&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J60="indice",$K$2&amp;"["&amp;H60&amp;"]",IF(J60="pnl","  pnl="&amp;G60,"  num="&amp;F60))))</f>
+        <v xml:space="preserve">  pnl=pnl1; pnl2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B61">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ca="1" si="3"/>
+        <v>9279</v>
+      </c>
+      <c r="E61">
+        <f t="shared" ca="1" si="4"/>
+        <v>739930</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>4,5 y 9; 9279; 739930</v>
+      </c>
+      <c r="G61" t="str">
+        <f>VLOOKUP(H61,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H61">
+        <v>11</v>
+      </c>
+      <c r="I61" t="str">
+        <f>VLOOKUP(H61,signos1!$A$1:$B$12,2,FALSE)</f>
+        <v>piscis</v>
+      </c>
+      <c r="J61" t="s">
         <v>126</v>
       </c>
-      <c r="D36" t="str">
-        <f>IF(C36="es","  "&amp;B36&amp;"_"&amp;C36&amp;"="&amp;VLOOKUP(B36&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C36="en","  "&amp;B36&amp;"_"&amp;C36&amp;"="&amp;VLOOKUP(B36&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A36&amp;"]"))</f>
+      <c r="K61" t="str">
+        <f>IF(J61="es","  "&amp;I61&amp;"_"&amp;J61&amp;"="&amp;VLOOKUP(I61&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J61="en","  "&amp;I61&amp;"_"&amp;J61&amp;"="&amp;VLOOKUP(I61&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J61="indice",$K$2&amp;"["&amp;H61&amp;"]",IF(J61="pnl","  pnl="&amp;G61,"  num="&amp;F61))))</f>
         <v xml:space="preserve">  piscis_es=Carga las baterías y asegúrate que tu apariencia es la mejor. Cuando se te vengan encima nuevas responsabilidades no temas Eres más que capaz de asumirlas y habrá alguien también dispuesto a echarte una mano si hace falta. Se acabó la diversión por un rato debes dedicarte ahora a un antiguo y duro trabajo. Actúa y recoge los beneficios. Necesitan tiempo y paciencia.</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C62">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ca="1" si="3"/>
+        <v>2659</v>
+      </c>
+      <c r="E62">
+        <f t="shared" ca="1" si="4"/>
+        <v>871274</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>2,6 y 8; 2659; 871274</v>
+      </c>
+      <c r="G62" t="str">
+        <f>VLOOKUP(H62,signos1!$A$1:$C$12,3,FALSE)</f>
+        <v>pnl1; pnl2</v>
+      </c>
+      <c r="H62">
         <v>11</v>
       </c>
-      <c r="B37" t="str">
-        <f>VLOOKUP(A37,signos1!$A$1:$B$12,2,FALSE)</f>
+      <c r="I62" t="str">
+        <f>VLOOKUP(H62,signos1!$A$1:$B$12,2,FALSE)</f>
         <v>piscis</v>
       </c>
-      <c r="C37" t="s">
+      <c r="J62" t="s">
         <v>432</v>
       </c>
-      <c r="D37" t="str">
-        <f>IF(C37="es","  "&amp;B37&amp;"_"&amp;C37&amp;"="&amp;VLOOKUP(B37&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(C37="en","  "&amp;B37&amp;"_"&amp;C37&amp;"="&amp;VLOOKUP(B37&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),$D$1&amp;"["&amp;A37&amp;"]"))</f>
+      <c r="K62" t="str">
+        <f>IF(J62="es","  "&amp;I62&amp;"_"&amp;J62&amp;"="&amp;VLOOKUP(I62&amp;"_"&amp;"diario",es!$A$3:$B$154,2,FALSE),IF(J62="en","  "&amp;I62&amp;"_"&amp;J62&amp;"="&amp;VLOOKUP(I62&amp;"_"&amp;"diario",en!$A$1:$B$152,2,FALSE),IF(J62="indice",$K$2&amp;"["&amp;H62&amp;"]",IF(J62="pnl","  pnl="&amp;G62,"  num="&amp;F62))))</f>
         <v xml:space="preserve">  piscis_en=Charge the batteries and make sure your appearance is the best. When new responsibilities come to you, do not fear. You are more than capable of assuming them and there will be someone willing to lend a hand if necessary. The fun is over for a while now you must dedicate yourself to an old and hard work. Acts and collects the benefits. They need time and patience.</v>
       </c>
     </row>

</xml_diff>